<commit_message>
Fixed the issue with smaller table load.
</commit_message>
<xml_diff>
--- a/agents/data/RMO_Agentic AI_train_test.xlsx
+++ b/agents/data/RMO_Agentic AI_train_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://noconline.sharepoint.com/sites/Digital-Conceptualisationteam/Shared Documents/General/005 In-Flight/UC - RMO Agentic AI/02 Colab/01 Oil well test monitoring/Data/anonymized data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AKE102\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{82BBFAFE-A5F1-4F36-A4C1-A0DCD116C636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1EB7A7-F288-48E1-955A-72287867C142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{B7CE08A2-946C-44C5-86BB-F8C8E6105459}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7CE08A2-946C-44C5-86BB-F8C8E6105459}"/>
   </bookViews>
   <sheets>
     <sheet name="cheetah-20" sheetId="2" r:id="rId1"/>
@@ -491,25 +491,237 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="124">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -630,14 +842,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -707,6 +911,14 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -836,6 +1048,25 @@
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3320,130 +3551,130 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FF884EF-F132-45B8-B7AF-85513D98C6A3}" name="Table1" displayName="Table1" ref="A1:W45" totalsRowShown="0" headerRowDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FF884EF-F132-45B8-B7AF-85513D98C6A3}" name="Table1" displayName="Table1" ref="A1:W45" headerRowDxfId="123">
   <autoFilter ref="A1:W45" xr:uid="{2FF884EF-F132-45B8-B7AF-85513D98C6A3}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{6A2A1B97-B6B7-445B-9091-A5CF117FE677}" name="Date" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{FA1CCB92-7779-4A10-A45A-CFA3AD045727}" name="Well Name" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{7D57D016-ED65-4BCE-B9B0-B57745BA116A}" name="WT LIQ" dataDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{42A6F4E2-B7AD-4F13-A611-E1DE3C00E4A1}" name="WT Oil" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{9A6E0C9E-E903-4C60-B248-5AF0C74E5C2A}" name="WT THP" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{8D6C6635-124F-46B2-B978-477EAC27E088}" name="WT WCT" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{9DD983B0-6C0F-461F-8350-6AA593B0B6C4}" name="Z1 BHP" dataDxfId="58"/>
-    <tableColumn id="8" xr3:uid="{56E6EB02-2D26-48D7-80A3-108DE753CFFA}" name="Z2 BHP" dataDxfId="57"/>
-    <tableColumn id="9" xr3:uid="{562FF221-B883-4B3D-B014-83D9FAD07247}" name="Z3 BHP" dataDxfId="56"/>
-    <tableColumn id="10" xr3:uid="{70C1F98E-16EE-41DF-AE92-7D5B87052AE2}" name="Column1" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{BC6E6709-167E-41F7-8275-72A459AC20F6}" name="Delta Liquid" dataDxfId="54">
+    <tableColumn id="1" xr3:uid="{6A2A1B97-B6B7-445B-9091-A5CF117FE677}" name="Date" totalsRowLabel="Total" dataDxfId="122" totalsRowDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{FA1CCB92-7779-4A10-A45A-CFA3AD045727}" name="Well Name" dataDxfId="121" totalsRowDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{7D57D016-ED65-4BCE-B9B0-B57745BA116A}" name="WT LIQ" dataDxfId="120" totalsRowDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{42A6F4E2-B7AD-4F13-A611-E1DE3C00E4A1}" name="WT Oil" dataDxfId="119" totalsRowDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{9A6E0C9E-E903-4C60-B248-5AF0C74E5C2A}" name="WT THP" dataDxfId="118" totalsRowDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{8D6C6635-124F-46B2-B978-477EAC27E088}" name="WT WCT" dataDxfId="117" totalsRowDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{9DD983B0-6C0F-461F-8350-6AA593B0B6C4}" name="Z1 BHP" dataDxfId="116" totalsRowDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{56E6EB02-2D26-48D7-80A3-108DE753CFFA}" name="Z2 BHP" dataDxfId="115" totalsRowDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{562FF221-B883-4B3D-B014-83D9FAD07247}" name="Z3 BHP" dataDxfId="114" totalsRowDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{70C1F98E-16EE-41DF-AE92-7D5B87052AE2}" name="Column1" dataDxfId="113" totalsRowDxfId="45"/>
+    <tableColumn id="11" xr3:uid="{BC6E6709-167E-41F7-8275-72A459AC20F6}" name="Delta Liquid" dataDxfId="112" totalsRowDxfId="46">
       <calculatedColumnFormula>C2-C1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2ABDBB1E-B953-4905-B9DB-EE284A5FA780}" name="Delta Oil" dataDxfId="53">
+    <tableColumn id="12" xr3:uid="{2ABDBB1E-B953-4905-B9DB-EE284A5FA780}" name="Delta Oil" dataDxfId="111" totalsRowDxfId="47">
       <calculatedColumnFormula>D2-D1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{A0FBA584-858D-4FAB-8FEC-62FCF028A5CB}" name="Delta THP" dataDxfId="52">
+    <tableColumn id="13" xr3:uid="{A0FBA584-858D-4FAB-8FEC-62FCF028A5CB}" name="Delta THP" dataDxfId="110" totalsRowDxfId="48">
       <calculatedColumnFormula>E2-E1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{4C13498F-976E-4626-B857-E87C14424ABF}" name="Delta WCT" dataDxfId="51">
+    <tableColumn id="14" xr3:uid="{4C13498F-976E-4626-B857-E87C14424ABF}" name="Delta WCT" dataDxfId="109" totalsRowDxfId="49">
       <calculatedColumnFormula>F2-F1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{3ED94272-405E-4F19-ACD1-34B3EF12EC2E}" name="Delta Z1 BHP" dataDxfId="50">
+    <tableColumn id="15" xr3:uid="{3ED94272-405E-4F19-ACD1-34B3EF12EC2E}" name="Delta Z1 BHP" dataDxfId="108" totalsRowDxfId="50">
       <calculatedColumnFormula>G2-G1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{8FEF217A-62E2-4ECF-8672-7D0229074DA2}" name="Delta Z2 BHP" dataDxfId="49">
+    <tableColumn id="16" xr3:uid="{8FEF217A-62E2-4ECF-8672-7D0229074DA2}" name="Delta Z2 BHP" dataDxfId="107" totalsRowDxfId="51">
       <calculatedColumnFormula>H2-H1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{06C5CD45-22A7-4E33-B900-71410FDC8E83}" name="Delta Z3BHP" dataDxfId="48">
+    <tableColumn id="17" xr3:uid="{06C5CD45-22A7-4E33-B900-71410FDC8E83}" name="Delta Z3BHP" dataDxfId="106" totalsRowDxfId="52">
       <calculatedColumnFormula>I2-I1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{85816F8E-AC9B-4B38-AFA1-E656F592840B}" name="Column2" dataDxfId="47"/>
-    <tableColumn id="19" xr3:uid="{6088AE26-02FD-47CD-9D4B-CFD6F941C801}" name="Decline Curve" dataDxfId="46"/>
-    <tableColumn id="20" xr3:uid="{5DFD1664-C0B0-4674-9FD3-44B5F7C8163D}" name="Zonal Configuration" dataDxfId="45"/>
-    <tableColumn id="21" xr3:uid="{F357CDC0-C987-46C0-AA93-BF59DFB517C7}" name="Engineer Interp" dataDxfId="44"/>
-    <tableColumn id="22" xr3:uid="{7E882BF6-3294-4A82-8E01-1306D2E9B6AD}" name="Engineer Action" dataDxfId="43"/>
-    <tableColumn id="23" xr3:uid="{A5C09C18-B1AD-4FC1-9773-31C2FBFDD2C3}" name="Notification" dataDxfId="42"/>
+    <tableColumn id="18" xr3:uid="{85816F8E-AC9B-4B38-AFA1-E656F592840B}" name="Column2" dataDxfId="105" totalsRowDxfId="53"/>
+    <tableColumn id="19" xr3:uid="{6088AE26-02FD-47CD-9D4B-CFD6F941C801}" name="Decline Curve" dataDxfId="104" totalsRowDxfId="54"/>
+    <tableColumn id="20" xr3:uid="{5DFD1664-C0B0-4674-9FD3-44B5F7C8163D}" name="Zonal Configuration" dataDxfId="103" totalsRowDxfId="55"/>
+    <tableColumn id="21" xr3:uid="{F357CDC0-C987-46C0-AA93-BF59DFB517C7}" name="Engineer Interp" dataDxfId="102" totalsRowDxfId="56"/>
+    <tableColumn id="22" xr3:uid="{7E882BF6-3294-4A82-8E01-1306D2E9B6AD}" name="Engineer Action" dataDxfId="101" totalsRowDxfId="57"/>
+    <tableColumn id="23" xr3:uid="{A5C09C18-B1AD-4FC1-9773-31C2FBFDD2C3}" name="Notification" totalsRowFunction="count" dataDxfId="100" totalsRowDxfId="58"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B721781C-3AE8-4665-88D4-0117DB5F8AEA}" name="Table2" displayName="Table2" ref="A1:W50" totalsRowShown="0" headerRowDxfId="18" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B721781C-3AE8-4665-88D4-0117DB5F8AEA}" name="Table2" displayName="Table2" ref="A1:W50" headerRowDxfId="99" dataDxfId="98">
   <autoFilter ref="A1:W50" xr:uid="{B721781C-3AE8-4665-88D4-0117DB5F8AEA}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{26BE2499-F992-4025-9E71-835D9B8B2972}" name="Date" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{0851A08C-3096-45B6-8EC9-9929587FB7EB}" name="Well Name" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{B5AA5BE5-23F7-41FF-8171-3009563F4D5C}" name="WT LIQ" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{C7576537-084B-4F18-96F3-53345D274ECD}" name="WT Oil" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{3900B91E-2668-49D1-9684-B9BEE98D8DC5}" name="WT THP" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{7BF02ADF-68B9-421B-924F-383A7962CDBB}" name="WT WCT" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{129E5A44-9045-425D-AB01-45E884B1651E}" name="Z1 BHP" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{6F369505-6AD1-4DF1-B5CE-DFF02543F40C}" name="Z2 BHP" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{83B9B20A-4ECA-4148-A1F4-A44A8E619DD4}" name="Z3 BHP" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{D99C22B1-9809-4B82-A6A7-EC3F786190BF}" name="Column1" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{4980D99E-4DD0-4E6F-B1AC-2C33E0D37C56}" name="Delta Liquid" dataDxfId="30">
+    <tableColumn id="1" xr3:uid="{26BE2499-F992-4025-9E71-835D9B8B2972}" name="Date" totalsRowLabel="Total" dataDxfId="97"/>
+    <tableColumn id="2" xr3:uid="{0851A08C-3096-45B6-8EC9-9929587FB7EB}" name="Well Name" dataDxfId="96" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{B5AA5BE5-23F7-41FF-8171-3009563F4D5C}" name="WT LIQ" dataDxfId="95" totalsRowDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{C7576537-084B-4F18-96F3-53345D274ECD}" name="WT Oil" dataDxfId="94" totalsRowDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{3900B91E-2668-49D1-9684-B9BEE98D8DC5}" name="WT THP" dataDxfId="93" totalsRowDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{7BF02ADF-68B9-421B-924F-383A7962CDBB}" name="WT WCT" dataDxfId="92" totalsRowDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{129E5A44-9045-425D-AB01-45E884B1651E}" name="Z1 BHP" dataDxfId="91" totalsRowDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{6F369505-6AD1-4DF1-B5CE-DFF02543F40C}" name="Z2 BHP" dataDxfId="90" totalsRowDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{83B9B20A-4ECA-4148-A1F4-A44A8E619DD4}" name="Z3 BHP" dataDxfId="89" totalsRowDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{D99C22B1-9809-4B82-A6A7-EC3F786190BF}" name="Column1" dataDxfId="88" totalsRowDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{4980D99E-4DD0-4E6F-B1AC-2C33E0D37C56}" name="Delta Liquid" dataDxfId="87" totalsRowDxfId="25">
       <calculatedColumnFormula>C2-C1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{88FBD97B-1F36-4F8C-9969-A1A1A924D482}" name="Delta Oil" dataDxfId="29">
+    <tableColumn id="12" xr3:uid="{88FBD97B-1F36-4F8C-9969-A1A1A924D482}" name="Delta Oil" dataDxfId="86" totalsRowDxfId="26">
       <calculatedColumnFormula>D2-D1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{51BCD2D7-71F2-4B17-96D0-CC66A1F49942}" name="Delta THP" dataDxfId="28">
+    <tableColumn id="13" xr3:uid="{51BCD2D7-71F2-4B17-96D0-CC66A1F49942}" name="Delta THP" dataDxfId="85" totalsRowDxfId="27">
       <calculatedColumnFormula>E2-E1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{1C7C4D54-21E7-4987-8CBE-544E29697F10}" name="Delta WCT" dataDxfId="27">
+    <tableColumn id="14" xr3:uid="{1C7C4D54-21E7-4987-8CBE-544E29697F10}" name="Delta WCT" dataDxfId="84" totalsRowDxfId="28">
       <calculatedColumnFormula>F2-F1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{446C6ED2-5E9C-4F25-A50A-7C972F8FAC3B}" name="Delta Z1 BHP" dataDxfId="26">
+    <tableColumn id="15" xr3:uid="{446C6ED2-5E9C-4F25-A50A-7C972F8FAC3B}" name="Delta Z1 BHP" dataDxfId="83" totalsRowDxfId="29">
       <calculatedColumnFormula>G2-G1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9AC659B6-AFF8-4D89-8100-78F55F21D103}" name="Delta Z2 BHP" dataDxfId="25">
+    <tableColumn id="16" xr3:uid="{9AC659B6-AFF8-4D89-8100-78F55F21D103}" name="Delta Z2 BHP" dataDxfId="82" totalsRowDxfId="30">
       <calculatedColumnFormula>H2-H1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{2DC31886-E1A3-411F-9437-140FF329540A}" name="Delta Z3BHP" dataDxfId="24">
+    <tableColumn id="17" xr3:uid="{2DC31886-E1A3-411F-9437-140FF329540A}" name="Delta Z3BHP" dataDxfId="81" totalsRowDxfId="31">
       <calculatedColumnFormula>I2-I1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{B0FB1F69-6ECF-4E2C-9270-7931A16AA272}" name="Column2" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{B0FB1F69-6ECF-4E2C-9270-7931A16AA272}" name="Column2" dataDxfId="80" totalsRowDxfId="32"/>
     <tableColumn id="19" xr3:uid="{E9387778-6258-40C5-9968-E36C12CF1D7D}" name="Decline Curve"/>
     <tableColumn id="20" xr3:uid="{8F2A89A7-93CC-4FDC-AE46-8F58337033A5}" name="Zonal Configuration"/>
-    <tableColumn id="21" xr3:uid="{B06B65AA-DB36-4B48-9E60-C7956941BD5D}" name="Engineer Interp" dataDxfId="22"/>
-    <tableColumn id="22" xr3:uid="{AEF68F5F-5DD8-4CD1-A521-2334C9615CDE}" name="Engineer Action" dataDxfId="21"/>
-    <tableColumn id="23" xr3:uid="{EF9ED262-3CD9-477A-A1F2-784414530601}" name="Notification" dataDxfId="20"/>
+    <tableColumn id="21" xr3:uid="{B06B65AA-DB36-4B48-9E60-C7956941BD5D}" name="Engineer Interp" dataDxfId="79" totalsRowDxfId="33"/>
+    <tableColumn id="22" xr3:uid="{AEF68F5F-5DD8-4CD1-A521-2334C9615CDE}" name="Engineer Action" dataDxfId="78" totalsRowDxfId="34"/>
+    <tableColumn id="23" xr3:uid="{EF9ED262-3CD9-477A-A1F2-784414530601}" name="Notification" totalsRowFunction="count" dataDxfId="77" totalsRowDxfId="35"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{091A1587-FBCF-4108-82CA-D15FD7DB7DF7}" name="Table3" displayName="Table3" ref="A1:W55" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{091A1587-FBCF-4108-82CA-D15FD7DB7DF7}" name="Table3" displayName="Table3" ref="A1:W55" headerRowDxfId="76">
   <autoFilter ref="A1:W55" xr:uid="{091A1587-FBCF-4108-82CA-D15FD7DB7DF7}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{FF7D051A-AF7B-4CD7-A0FE-ECEB091592D7}" name="Date" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{64C8DF5F-2AED-4C62-B5D3-C01569CE794A}" name="WellName" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{E8523D35-C390-49C2-AB45-6879D4B6D6D1}" name="WT LIQ" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{BEFC5705-64F1-4200-BAF0-F23B341253E6}" name="WT Oil" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{CB8BBD66-D9DB-4E58-8C5B-3BC75D85BD98}" name="WT THP" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{CB8A1938-D0EA-4F17-888F-075B94127F4C}" name="WT WCT" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{62A81805-CF9C-48DB-9AD3-F53565EA5555}" name="Z1 BHP" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{901F5709-676F-4479-8101-9C0DB3F973C3}" name="Z2 BHP" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{11AEC6B4-836C-464D-9C9F-020FB198F5FC}" name="Z3 BHP" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{43991539-37A6-4052-ADB5-70D06B29C33D}" name="Column1" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{76577A11-9DF2-4A06-9B57-23897BC59F4F}" name="Delta Liquid" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{FF7D051A-AF7B-4CD7-A0FE-ECEB091592D7}" name="Date" totalsRowLabel="Total" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{64C8DF5F-2AED-4C62-B5D3-C01569CE794A}" name="WellName" dataDxfId="74" totalsRowDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{E8523D35-C390-49C2-AB45-6879D4B6D6D1}" name="WT LIQ" dataDxfId="73" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{BEFC5705-64F1-4200-BAF0-F23B341253E6}" name="WT Oil" dataDxfId="72" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{CB8BBD66-D9DB-4E58-8C5B-3BC75D85BD98}" name="WT THP" dataDxfId="71" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{CB8A1938-D0EA-4F17-888F-075B94127F4C}" name="WT WCT" dataDxfId="70" totalsRowDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{62A81805-CF9C-48DB-9AD3-F53565EA5555}" name="Z1 BHP" dataDxfId="69" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{901F5709-676F-4479-8101-9C0DB3F973C3}" name="Z2 BHP" dataDxfId="68" totalsRowDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{11AEC6B4-836C-464D-9C9F-020FB198F5FC}" name="Z3 BHP" dataDxfId="67" totalsRowDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{43991539-37A6-4052-ADB5-70D06B29C33D}" name="Column1" dataDxfId="66" totalsRowDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{76577A11-9DF2-4A06-9B57-23897BC59F4F}" name="Delta Liquid" dataDxfId="65" totalsRowDxfId="9">
       <calculatedColumnFormula>C2-C1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{1F631ABE-79D8-40B9-8867-9B0F7A5C9F96}" name="Delta Oil" dataDxfId="6">
+    <tableColumn id="12" xr3:uid="{1F631ABE-79D8-40B9-8867-9B0F7A5C9F96}" name="Delta Oil" dataDxfId="64" totalsRowDxfId="10">
       <calculatedColumnFormula>D2-D1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{A9E93A22-C778-4D60-A856-1847131A9063}" name="Delta THP" dataDxfId="5">
+    <tableColumn id="13" xr3:uid="{A9E93A22-C778-4D60-A856-1847131A9063}" name="Delta THP" dataDxfId="63" totalsRowDxfId="11">
       <calculatedColumnFormula>E2-E1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{7BB3144F-DD2D-49E0-B696-0A804247AA0A}" name="Delta WCT" dataDxfId="4">
+    <tableColumn id="14" xr3:uid="{7BB3144F-DD2D-49E0-B696-0A804247AA0A}" name="Delta WCT" dataDxfId="62" totalsRowDxfId="12">
       <calculatedColumnFormula>F2-F1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{6D54DC35-F390-4BD1-A92E-990129B577BC}" name="Delta Z1 BHP" dataDxfId="3">
+    <tableColumn id="15" xr3:uid="{6D54DC35-F390-4BD1-A92E-990129B577BC}" name="Delta Z1 BHP" dataDxfId="61" totalsRowDxfId="13">
       <calculatedColumnFormula>G2-G1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{6E65DD41-BAD7-42AE-9E24-A3FF3AF73C4D}" name="Delta Z2 BHP" dataDxfId="2">
+    <tableColumn id="16" xr3:uid="{6E65DD41-BAD7-42AE-9E24-A3FF3AF73C4D}" name="Delta Z2 BHP" dataDxfId="60" totalsRowDxfId="14">
       <calculatedColumnFormula>H2-H1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{0175E5E9-80B8-4610-946D-572C25C6DE5A}" name="Delta Z3BHP" dataDxfId="1">
+    <tableColumn id="17" xr3:uid="{0175E5E9-80B8-4610-946D-572C25C6DE5A}" name="Delta Z3BHP" dataDxfId="59" totalsRowDxfId="15">
       <calculatedColumnFormula>I2-I1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{C85630ED-F921-43A6-8BE4-008BED0D010F}" name="Column2"/>
@@ -3451,7 +3682,7 @@
     <tableColumn id="20" xr3:uid="{DC36E30F-0A64-424F-88FD-E313CE688FD6}" name="Zonal Configuration"/>
     <tableColumn id="21" xr3:uid="{1109DFDF-B26B-49E8-B243-15CC528FBA53}" name="Engineer Interp"/>
     <tableColumn id="22" xr3:uid="{76F6A55C-F825-43DF-88BB-68D52FA12211}" name="Engineer Action"/>
-    <tableColumn id="23" xr3:uid="{099B4A9D-B6FE-4D2A-8043-411205F6E0CF}" name="Notification"/>
+    <tableColumn id="23" xr3:uid="{099B4A9D-B6FE-4D2A-8043-411205F6E0CF}" name="Notification" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3776,41 +4007,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE786F4-2E39-4A5D-A6C0-84B85921C631}">
   <dimension ref="A1:AE45"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="14.81640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.81640625" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.26953125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" hidden="1" customWidth="1"/>
+    <col min="7" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.453125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="16.453125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="16.81640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="16" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="13.54296875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="19.54296875" customWidth="1"/>
-    <col min="20" max="20" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="56.26953125" customWidth="1"/>
-    <col min="23" max="23" width="100.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.453125" customWidth="1"/>
-    <col min="25" max="25" width="14.81640625" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" customWidth="1"/>
+    <col min="20" max="20" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="56.28515625" customWidth="1"/>
+    <col min="23" max="23" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.42578125" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" customWidth="1"/>
     <col min="26" max="27" width="16" customWidth="1"/>
-    <col min="29" max="29" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="62.7265625" customWidth="1"/>
+    <col min="29" max="29" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="62.7109375" customWidth="1"/>
     <col min="31" max="31" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3881,7 +4112,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
         <v>45115</v>
       </c>
@@ -3947,7 +4178,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>45116</v>
       </c>
@@ -4022,7 +4253,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="39">
         <v>45117</v>
       </c>
@@ -4094,7 +4325,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="39">
         <v>45118</v>
       </c>
@@ -4167,7 +4398,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="39">
         <v>45138</v>
       </c>
@@ -4240,7 +4471,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="39">
         <v>45154</v>
       </c>
@@ -4313,7 +4544,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
         <v>45188</v>
       </c>
@@ -4386,7 +4617,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <v>45197</v>
       </c>
@@ -4459,7 +4690,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="39">
         <v>45205</v>
       </c>
@@ -4532,7 +4763,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
         <v>45220</v>
       </c>
@@ -4605,7 +4836,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
         <v>45277</v>
       </c>
@@ -4687,7 +4918,7 @@
       <c r="AD12" s="26"/>
       <c r="AE12" s="26"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="39">
         <v>45278</v>
       </c>
@@ -4768,7 +4999,7 @@
       <c r="AD13" s="26"/>
       <c r="AE13" s="26"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="39">
         <v>45279</v>
       </c>
@@ -4848,7 +5079,7 @@
       <c r="AD14" s="26"/>
       <c r="AE14" s="26"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="39">
         <v>45281</v>
       </c>
@@ -4929,7 +5160,7 @@
       <c r="AD15" s="26"/>
       <c r="AE15" s="26"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="39">
         <v>45282</v>
       </c>
@@ -5010,7 +5241,7 @@
       <c r="AD16" s="30"/>
       <c r="AE16" s="30"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="39">
         <v>45285</v>
       </c>
@@ -5091,7 +5322,7 @@
       <c r="AD17" s="31"/>
       <c r="AE17" s="31"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="39">
         <v>45286</v>
       </c>
@@ -5172,7 +5403,7 @@
       <c r="AD18" s="31"/>
       <c r="AE18" s="31"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="39">
         <v>45287</v>
       </c>
@@ -5253,7 +5484,7 @@
       <c r="AD19" s="31"/>
       <c r="AE19" s="31"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
         <v>45325</v>
       </c>
@@ -5335,7 +5566,7 @@
       <c r="AD20" s="26"/>
       <c r="AE20" s="26"/>
     </row>
-    <row r="21" spans="1:31" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>45363</v>
       </c>
@@ -5417,7 +5648,7 @@
       <c r="AD21" s="26"/>
       <c r="AE21" s="26"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
         <v>45376</v>
       </c>
@@ -5499,7 +5730,7 @@
       <c r="AD22" s="26"/>
       <c r="AE22" s="26"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="39">
         <v>45408</v>
       </c>
@@ -5580,7 +5811,7 @@
       <c r="AD23" s="26"/>
       <c r="AE23" s="26"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="39">
         <v>45425</v>
       </c>
@@ -5653,7 +5884,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="39">
         <v>45449</v>
       </c>
@@ -5726,7 +5957,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="39">
         <v>45495</v>
       </c>
@@ -5799,7 +6030,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="39">
         <v>45500</v>
       </c>
@@ -5872,7 +6103,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="39">
         <v>45513</v>
       </c>
@@ -5945,7 +6176,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="41">
         <v>45524</v>
       </c>
@@ -6019,7 +6250,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>45525</v>
       </c>
@@ -6093,7 +6324,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>45538</v>
       </c>
@@ -6167,7 +6398,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>45547</v>
       </c>
@@ -6241,7 +6472,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>45553</v>
       </c>
@@ -6315,7 +6546,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>45566</v>
       </c>
@@ -6389,7 +6620,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>45580</v>
       </c>
@@ -6463,7 +6694,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="42">
         <v>45608</v>
       </c>
@@ -6537,7 +6768,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="42">
         <v>45622</v>
       </c>
@@ -6611,7 +6842,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="42">
         <v>45625</v>
       </c>
@@ -6685,7 +6916,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="42">
         <v>45652</v>
       </c>
@@ -6759,7 +6990,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="42">
         <v>45679</v>
       </c>
@@ -6833,7 +7064,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="42">
         <v>45702</v>
       </c>
@@ -6907,7 +7138,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="42">
         <v>45707</v>
       </c>
@@ -6981,7 +7212,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="42">
         <v>45729</v>
       </c>
@@ -7055,7 +7286,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="42">
         <v>45755</v>
       </c>
@@ -7129,7 +7360,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="42">
         <v>45770</v>
       </c>
@@ -7483,39 +7714,39 @@
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S8" sqref="S8"/>
+      <selection pane="bottomLeft" activeCell="W50" sqref="A1:W50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="14.81640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.81640625" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.26953125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" hidden="1" customWidth="1"/>
+    <col min="7" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.453125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="16.453125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="16.81640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="16" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="5" style="9" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="19.54296875" customWidth="1"/>
-    <col min="20" max="20" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="56.26953125" customWidth="1"/>
-    <col min="23" max="23" width="100.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.453125" customWidth="1"/>
-    <col min="25" max="25" width="14.81640625" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" customWidth="1"/>
+    <col min="20" max="20" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="56.28515625" customWidth="1"/>
+    <col min="23" max="23" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.42578125" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" customWidth="1"/>
     <col min="26" max="27" width="16" customWidth="1"/>
-    <col min="29" max="29" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="62.7265625" customWidth="1"/>
+    <col min="29" max="29" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="62.7109375" customWidth="1"/>
     <col min="31" max="31" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7586,7 +7817,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45011</v>
       </c>
@@ -7651,7 +7882,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45012</v>
       </c>
@@ -7716,7 +7947,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45013</v>
       </c>
@@ -7778,7 +8009,7 @@
       <c r="V4" s="22"/>
       <c r="W4" s="22"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45014</v>
       </c>
@@ -7840,7 +8071,7 @@
       <c r="U5" s="22"/>
       <c r="V5" s="22"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45015</v>
       </c>
@@ -7903,7 +8134,7 @@
       <c r="V6" s="24"/>
       <c r="W6" s="24"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45024</v>
       </c>
@@ -7966,7 +8197,7 @@
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45043</v>
       </c>
@@ -8029,7 +8260,7 @@
       <c r="V8" s="24"/>
       <c r="W8" s="24"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45056</v>
       </c>
@@ -8092,7 +8323,7 @@
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45089</v>
       </c>
@@ -8163,7 +8394,7 @@
       <c r="AD10" s="26"/>
       <c r="AE10" s="26"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45095</v>
       </c>
@@ -8234,7 +8465,7 @@
       <c r="AD11" s="26"/>
       <c r="AE11" s="26"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45111</v>
       </c>
@@ -8304,7 +8535,7 @@
       <c r="AD12" s="26"/>
       <c r="AE12" s="26"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45139</v>
       </c>
@@ -8375,7 +8606,7 @@
       <c r="AD13" s="26"/>
       <c r="AE13" s="26"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45154</v>
       </c>
@@ -8446,7 +8677,7 @@
       <c r="AD14" s="30"/>
       <c r="AE14" s="30"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45188</v>
       </c>
@@ -8517,7 +8748,7 @@
       <c r="AD15" s="31"/>
       <c r="AE15" s="31"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45198</v>
       </c>
@@ -8588,7 +8819,7 @@
       <c r="AD16" s="31"/>
       <c r="AE16" s="31"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45214</v>
       </c>
@@ -8659,7 +8890,7 @@
       <c r="AD17" s="31"/>
       <c r="AE17" s="31"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45284</v>
       </c>
@@ -8730,7 +8961,7 @@
       <c r="AD18" s="26"/>
       <c r="AE18" s="26"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45322</v>
       </c>
@@ -8802,7 +9033,7 @@
       <c r="AD19" s="26"/>
       <c r="AE19" s="26"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45324</v>
       </c>
@@ -8873,7 +9104,7 @@
       <c r="AD20" s="26"/>
       <c r="AE20" s="26"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45396</v>
       </c>
@@ -8936,7 +9167,7 @@
       <c r="V21" s="24"/>
       <c r="W21" s="24"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45418</v>
       </c>
@@ -8999,7 +9230,7 @@
       <c r="V22" s="24"/>
       <c r="W22" s="24"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45419</v>
       </c>
@@ -9062,7 +9293,7 @@
       <c r="V23" s="24"/>
       <c r="W23" s="24"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45420</v>
       </c>
@@ -9125,7 +9356,7 @@
       <c r="V24" s="24"/>
       <c r="W24" s="24"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45421</v>
       </c>
@@ -9188,7 +9419,7 @@
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45423</v>
       </c>
@@ -9252,7 +9483,7 @@
       <c r="V26" s="20"/>
       <c r="W26" s="24"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45424</v>
       </c>
@@ -9316,7 +9547,7 @@
       <c r="V27" s="20"/>
       <c r="W27" s="24"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45426</v>
       </c>
@@ -9380,7 +9611,7 @@
       <c r="V28" s="20"/>
       <c r="W28" s="24"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45428</v>
       </c>
@@ -9444,7 +9675,7 @@
       <c r="V29" s="20"/>
       <c r="W29" s="24"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45429</v>
       </c>
@@ -9508,7 +9739,7 @@
       <c r="V30" s="20"/>
       <c r="W30" s="24"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45431</v>
       </c>
@@ -9572,7 +9803,7 @@
       <c r="V31" s="20"/>
       <c r="W31" s="24"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45473</v>
       </c>
@@ -9636,7 +9867,7 @@
       <c r="V32" s="20"/>
       <c r="W32" s="24"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45499</v>
       </c>
@@ -9700,7 +9931,7 @@
       <c r="V33" s="20"/>
       <c r="W33" s="24"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>45511</v>
       </c>
@@ -9764,7 +9995,7 @@
       <c r="V34" s="20"/>
       <c r="W34" s="24"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>45531</v>
       </c>
@@ -9828,7 +10059,7 @@
       <c r="V35" s="20"/>
       <c r="W35" s="24"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>45537</v>
       </c>
@@ -9892,7 +10123,7 @@
       <c r="V36" s="20"/>
       <c r="W36" s="24"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>45546</v>
       </c>
@@ -9956,7 +10187,7 @@
       <c r="V37" s="20"/>
       <c r="W37" s="24"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>45554</v>
       </c>
@@ -10020,7 +10251,7 @@
       <c r="V38" s="20"/>
       <c r="W38" s="24"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>45564</v>
       </c>
@@ -10084,7 +10315,7 @@
       <c r="V39" s="20"/>
       <c r="W39" s="24"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>45585</v>
       </c>
@@ -10148,7 +10379,7 @@
       <c r="V40" s="20"/>
       <c r="W40" s="24"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>45602</v>
       </c>
@@ -10212,7 +10443,7 @@
       <c r="V41" s="20"/>
       <c r="W41" s="24"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45611</v>
       </c>
@@ -10276,7 +10507,7 @@
       <c r="V42" s="20"/>
       <c r="W42" s="24"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45622</v>
       </c>
@@ -10336,7 +10567,7 @@
       <c r="V43" s="9"/>
       <c r="W43" s="9"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>45650</v>
       </c>
@@ -10396,7 +10627,7 @@
       <c r="V44" s="9"/>
       <c r="W44" s="9"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45672</v>
       </c>
@@ -10456,7 +10687,7 @@
       <c r="V45" s="9"/>
       <c r="W45" s="9"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45687</v>
       </c>
@@ -10516,7 +10747,7 @@
       <c r="V46" s="9"/>
       <c r="W46" s="9"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45703</v>
       </c>
@@ -10576,7 +10807,7 @@
       <c r="V47" s="9"/>
       <c r="W47" s="9"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45719</v>
       </c>
@@ -10636,7 +10867,7 @@
       <c r="V48" s="9"/>
       <c r="W48" s="9"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45739</v>
       </c>
@@ -10693,7 +10924,7 @@
         <v>-190</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>45757</v>
       </c>
@@ -11111,35 +11342,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9682B22-FDD1-4027-970E-00CB8D045BD0}">
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T15" sqref="T15"/>
+      <selection pane="bottomLeft" sqref="A1:W55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="14.81640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.81640625" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.26953125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" hidden="1" customWidth="1"/>
+    <col min="7" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.453125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="16.453125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="16.81640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="16" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="13.54296875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="19.54296875" customWidth="1"/>
-    <col min="20" max="20" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="56.26953125" customWidth="1"/>
-    <col min="23" max="23" width="100.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" customWidth="1"/>
+    <col min="20" max="20" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="56.28515625" customWidth="1"/>
+    <col min="23" max="23" width="110.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -11210,7 +11441,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45039</v>
       </c>
@@ -11276,7 +11507,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45040</v>
       </c>
@@ -11338,7 +11569,7 @@
       <c r="V3" s="22"/>
       <c r="W3" s="22"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45041</v>
       </c>
@@ -11400,7 +11631,7 @@
       <c r="V4" s="22"/>
       <c r="W4" s="22"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45042</v>
       </c>
@@ -11462,7 +11693,7 @@
       <c r="U5" s="22"/>
       <c r="V5" s="22"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45055</v>
       </c>
@@ -11526,7 +11757,7 @@
       <c r="V6" s="24"/>
       <c r="W6" s="24"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45088</v>
       </c>
@@ -11590,7 +11821,7 @@
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45093</v>
       </c>
@@ -11654,7 +11885,7 @@
       <c r="V8" s="24"/>
       <c r="W8" s="24"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45094</v>
       </c>
@@ -11718,7 +11949,7 @@
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45112</v>
       </c>
@@ -11782,7 +12013,7 @@
       <c r="V10" s="24"/>
       <c r="W10" s="24"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45139</v>
       </c>
@@ -11846,7 +12077,7 @@
       <c r="V11" s="24"/>
       <c r="W11" s="24"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45159</v>
       </c>
@@ -11910,7 +12141,7 @@
       <c r="V12" s="20"/>
       <c r="W12" s="24"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45189</v>
       </c>
@@ -11974,7 +12205,7 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45198</v>
       </c>
@@ -12038,7 +12269,7 @@
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45215</v>
       </c>
@@ -12102,7 +12333,7 @@
       <c r="V15" s="24"/>
       <c r="W15" s="24"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45276</v>
       </c>
@@ -12166,7 +12397,7 @@
       <c r="V16" s="24"/>
       <c r="W16" s="24"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45277</v>
       </c>
@@ -12230,7 +12461,7 @@
       <c r="V17" s="24"/>
       <c r="W17" s="24"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45279</v>
       </c>
@@ -12294,7 +12525,7 @@
       <c r="V18" s="24"/>
       <c r="W18" s="24"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45280</v>
       </c>
@@ -12358,7 +12589,7 @@
       <c r="V19" s="20"/>
       <c r="W19" s="24"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45281</v>
       </c>
@@ -12422,7 +12653,7 @@
       <c r="V20" s="20"/>
       <c r="W20" s="24"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45282</v>
       </c>
@@ -12486,7 +12717,7 @@
       <c r="V21" s="20"/>
       <c r="W21" s="24"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45285</v>
       </c>
@@ -12550,7 +12781,7 @@
       <c r="V22" s="20"/>
       <c r="W22" s="24"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45286</v>
       </c>
@@ -12614,7 +12845,7 @@
       <c r="V23" s="20"/>
       <c r="W23" s="24"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45287</v>
       </c>
@@ -12678,7 +12909,7 @@
       <c r="V24" s="20"/>
       <c r="W24" s="24"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45325</v>
       </c>
@@ -12742,7 +12973,7 @@
       <c r="V25" s="20"/>
       <c r="W25" s="24"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45338</v>
       </c>
@@ -12806,7 +13037,7 @@
       <c r="V26" s="20"/>
       <c r="W26" s="24"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45362</v>
       </c>
@@ -12870,7 +13101,7 @@
       <c r="V27" s="20"/>
       <c r="W27" s="24"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45365</v>
       </c>
@@ -12934,7 +13165,7 @@
       <c r="V28" s="20"/>
       <c r="W28" s="24"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45393</v>
       </c>
@@ -12998,7 +13229,7 @@
       <c r="V29" s="20"/>
       <c r="W29" s="24"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45422</v>
       </c>
@@ -13062,7 +13293,7 @@
       <c r="V30" s="20"/>
       <c r="W30" s="24"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45449</v>
       </c>
@@ -13126,7 +13357,7 @@
       <c r="V31" s="20"/>
       <c r="W31" s="24"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45454</v>
       </c>
@@ -13190,7 +13421,7 @@
       <c r="V32" s="20"/>
       <c r="W32" s="24"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45456</v>
       </c>
@@ -13254,7 +13485,7 @@
       <c r="V33" s="20"/>
       <c r="W33" s="24"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>45458</v>
       </c>
@@ -13318,7 +13549,7 @@
       <c r="V34" s="20"/>
       <c r="W34" s="24"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>45460</v>
       </c>
@@ -13382,7 +13613,7 @@
       <c r="V35" s="20"/>
       <c r="W35" s="24"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>45462</v>
       </c>
@@ -13442,7 +13673,7 @@
       <c r="V36" s="9"/>
       <c r="W36" s="9"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>45465</v>
       </c>
@@ -13502,7 +13733,7 @@
       <c r="V37" s="9"/>
       <c r="W37" s="9"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>45467</v>
       </c>
@@ -13562,7 +13793,7 @@
       <c r="V38" s="9"/>
       <c r="W38" s="9"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>45476</v>
       </c>
@@ -13622,7 +13853,7 @@
       <c r="V39" s="9"/>
       <c r="W39" s="9"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>45496</v>
       </c>
@@ -13682,7 +13913,7 @@
       <c r="V40" s="9"/>
       <c r="W40" s="9"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>45503</v>
       </c>
@@ -13739,7 +13970,7 @@
         <v>-60</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45509</v>
       </c>
@@ -13796,7 +14027,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45545</v>
       </c>
@@ -13853,7 +14084,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>45557</v>
       </c>
@@ -13910,7 +14141,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45576</v>
       </c>
@@ -13967,7 +14198,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45578</v>
       </c>
@@ -14024,7 +14255,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45594</v>
       </c>
@@ -14081,7 +14312,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45610</v>
       </c>
@@ -14138,7 +14369,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45625</v>
       </c>
@@ -14195,7 +14426,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>45651</v>
       </c>
@@ -14252,7 +14483,7 @@
         <v>-110</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>45673</v>
       </c>
@@ -14309,7 +14540,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45685</v>
       </c>
@@ -14366,7 +14597,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45701</v>
       </c>
@@ -14423,7 +14654,7 @@
         <v>-270</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>45717</v>
       </c>
@@ -14480,7 +14711,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>45759</v>
       </c>
@@ -14971,7 +15202,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -14987,39 +15218,39 @@
       <selection pane="bottomLeft" activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7265625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.54296875" customWidth="1"/>
-    <col min="20" max="20" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="56.26953125" customWidth="1"/>
-    <col min="23" max="23" width="100.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.453125" customWidth="1"/>
-    <col min="25" max="25" width="14.81640625" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" customWidth="1"/>
+    <col min="20" max="20" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="56.28515625" customWidth="1"/>
+    <col min="23" max="23" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.42578125" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" customWidth="1"/>
     <col min="26" max="27" width="16" customWidth="1"/>
-    <col min="29" max="29" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="62.7265625" customWidth="1"/>
+    <col min="29" max="29" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="62.7109375" customWidth="1"/>
     <col min="31" max="31" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -15085,7 +15316,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>45410</v>
       </c>
@@ -15142,7 +15373,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>45411</v>
       </c>
@@ -15199,7 +15430,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>45412</v>
       </c>
@@ -15253,7 +15484,7 @@
       <c r="V4" s="24"/>
       <c r="W4" s="24"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>45413</v>
       </c>
@@ -15307,7 +15538,7 @@
       <c r="V5" s="24"/>
       <c r="W5" s="9"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>45414</v>
       </c>
@@ -15361,7 +15592,7 @@
       <c r="V6" s="24"/>
       <c r="W6" s="24"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>45417</v>
       </c>
@@ -15415,7 +15646,7 @@
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>45429</v>
       </c>
@@ -15469,7 +15700,7 @@
       <c r="V8" s="24"/>
       <c r="W8" s="24"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>45440</v>
       </c>
@@ -15523,7 +15754,7 @@
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>45448</v>
       </c>
@@ -15577,7 +15808,7 @@
       <c r="V10" s="24"/>
       <c r="W10" s="24"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>45489</v>
       </c>
@@ -15631,7 +15862,7 @@
       <c r="V11" s="24"/>
       <c r="W11" s="24"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>45508</v>
       </c>
@@ -15694,7 +15925,7 @@
       <c r="V12" s="24"/>
       <c r="W12" s="24"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>45541</v>
       </c>
@@ -15757,7 +15988,7 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>45552</v>
       </c>
@@ -15820,7 +16051,7 @@
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>45565</v>
       </c>
@@ -15884,7 +16115,7 @@
       <c r="V15" s="20"/>
       <c r="W15" s="24"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>45568</v>
       </c>
@@ -15947,7 +16178,7 @@
       <c r="V16" s="24"/>
       <c r="W16" s="24"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>45580</v>
       </c>
@@ -16010,7 +16241,7 @@
       <c r="V17" s="24"/>
       <c r="W17" s="24"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>45586</v>
       </c>
@@ -16073,7 +16304,7 @@
       <c r="V18" s="24"/>
       <c r="W18" s="24"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>45596</v>
       </c>
@@ -16137,7 +16368,7 @@
       <c r="V19" s="20"/>
       <c r="W19" s="24"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>45611</v>
       </c>
@@ -16201,7 +16432,7 @@
       <c r="V20" s="20"/>
       <c r="W20" s="24"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>45623</v>
       </c>
@@ -16265,7 +16496,7 @@
       <c r="V21" s="20"/>
       <c r="W21" s="24"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>45629</v>
       </c>
@@ -16329,7 +16560,7 @@
       <c r="V22" s="20"/>
       <c r="W22" s="24"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>45643</v>
       </c>
@@ -16393,7 +16624,7 @@
       <c r="V23" s="20"/>
       <c r="W23" s="24"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>45670</v>
       </c>
@@ -16457,7 +16688,7 @@
       <c r="V24" s="20"/>
       <c r="W24" s="24"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>45690</v>
       </c>
@@ -16521,7 +16752,7 @@
       <c r="V25" s="20"/>
       <c r="W25" s="24"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>45692</v>
       </c>
@@ -16585,7 +16816,7 @@
       <c r="V26" s="20"/>
       <c r="W26" s="24"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>45695</v>
       </c>
@@ -16649,7 +16880,7 @@
       <c r="V27" s="20"/>
       <c r="W27" s="24"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>45698</v>
       </c>
@@ -16713,7 +16944,7 @@
       <c r="V28" s="20"/>
       <c r="W28" s="24"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>45700</v>
       </c>
@@ -16777,7 +17008,7 @@
       <c r="V29" s="20"/>
       <c r="W29" s="24"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>45718</v>
       </c>
@@ -16841,7 +17072,7 @@
       <c r="V30" s="20"/>
       <c r="W30" s="24"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>45762</v>
       </c>
@@ -16905,7 +17136,7 @@
       <c r="V31" s="20"/>
       <c r="W31" s="24"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>45766</v>
       </c>
@@ -16969,7 +17200,7 @@
       <c r="V32" s="20"/>
       <c r="W32" s="24"/>
     </row>
-    <row r="33" spans="10:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J33" s="24"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
@@ -16985,7 +17216,7 @@
       <c r="V33" s="20"/>
       <c r="W33" s="24"/>
     </row>
-    <row r="58" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="58" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X58" s="26"/>
       <c r="Y58" s="26"/>
       <c r="Z58" s="26"/>
@@ -16995,7 +17226,7 @@
       <c r="AD58" s="26"/>
       <c r="AE58" s="26"/>
     </row>
-    <row r="59" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="59" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X59" s="26"/>
       <c r="Y59" s="26"/>
       <c r="Z59" s="26"/>
@@ -17005,7 +17236,7 @@
       <c r="AD59" s="26"/>
       <c r="AE59" s="26"/>
     </row>
-    <row r="60" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="60" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X60" s="26"/>
       <c r="Z60" s="26"/>
       <c r="AA60" s="26"/>
@@ -17014,7 +17245,7 @@
       <c r="AD60" s="26"/>
       <c r="AE60" s="26"/>
     </row>
-    <row r="61" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="61" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X61" s="26"/>
       <c r="Y61" s="32" t="s">
         <v>64</v>
@@ -17026,7 +17257,7 @@
       <c r="AD61" s="26"/>
       <c r="AE61" s="26"/>
     </row>
-    <row r="62" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="62" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X62" s="26"/>
       <c r="Y62" s="27" t="s">
         <v>59</v>
@@ -17050,7 +17281,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="63" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X63" s="26"/>
       <c r="Y63" s="28" t="s">
         <v>42</v>
@@ -17077,7 +17308,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="64" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X64" s="26"/>
       <c r="Y64" s="28" t="s">
         <v>43</v>
@@ -17104,7 +17335,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="65" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X65" s="26"/>
       <c r="Y65" s="28" t="s">
         <v>44</v>
@@ -17131,7 +17362,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="66" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X66" s="26"/>
       <c r="Y66" s="26"/>
       <c r="Z66" s="26"/>
@@ -17141,7 +17372,7 @@
       <c r="AD66" s="26"/>
       <c r="AE66" s="26"/>
     </row>
-    <row r="67" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="67" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X67" s="26"/>
       <c r="Y67" s="32" t="s">
         <v>71</v>
@@ -17153,7 +17384,7 @@
       <c r="AD67" s="26"/>
       <c r="AE67" s="26"/>
     </row>
-    <row r="68" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="68" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X68" s="26"/>
       <c r="Y68" s="26" t="s">
         <v>72</v>
@@ -17165,7 +17396,7 @@
       <c r="AD68" s="26"/>
       <c r="AE68" s="26"/>
     </row>
-    <row r="69" spans="24:31" x14ac:dyDescent="0.35">
+    <row r="69" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X69" s="26"/>
       <c r="Y69" s="26"/>
       <c r="Z69" s="26"/>

</xml_diff>